<commit_message>
Fixes to imports (pyqt6)
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -36149,7 +36149,7 @@
         <v>74</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>375</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3">
@@ -36437,31 +36437,31 @@
         <v/>
       </c>
       <c r="D4" s="6" t="n">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="E4" s="6" t="n">
         <v>40</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4" s="6" t="n">
         <v>3.5</v>
       </c>
       <c r="H4" s="6" t="n">
-        <v>0.1251051490908961</v>
+        <v>0.09762957106432885</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>33.358750254646</v>
+        <v>33.14057753777865</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>81.6112196904521</v>
+        <v>81.45891194576367</v>
       </c>
       <c r="K4" s="6" t="n">
-        <v>34.8983773635332</v>
+        <v>34.87566493717577</v>
       </c>
       <c r="L4" s="6" t="n">
-        <v>30.9558712909312</v>
+        <v>20.63724752728747</v>
       </c>
       <c r="M4" s="6" t="n">
         <v>1.448572791205265</v>
@@ -36481,31 +36481,31 @@
         <v/>
       </c>
       <c r="D5" s="6" t="n">
-        <v>314</v>
+        <v>224</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="6" t="n">
         <v>3.5</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>0.1322048449492725</v>
+        <v>-0.00711632987305845</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>32.53806183760429</v>
+        <v>32.07704468651275</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>76.93882658115621</v>
+        <v>76.24284633995511</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>34.83184605125393</v>
+        <v>34.68726983077948</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>25.79655940910934</v>
+        <v>0</v>
       </c>
       <c r="M5" s="6" t="n">
         <v>1.448572791205265</v>

</xml_diff>

<commit_message>
working version 1.2 - cleaned up excel file
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -74213,13 +74213,13 @@
         </is>
       </c>
       <c r="B2" s="6" t="n">
-        <v>29.14000000000004</v>
+        <v>26.89000000000004</v>
       </c>
       <c r="C2" s="6" t="n">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3">
@@ -74229,10 +74229,10 @@
         </is>
       </c>
       <c r="B3" s="6" t="n">
-        <v>28.16000000000003</v>
+        <v>30.67000000000002</v>
       </c>
       <c r="C3" s="6" t="n">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
@@ -74242,10 +74242,10 @@
         </is>
       </c>
       <c r="B4" s="6" t="n">
-        <v>29.96000000000004</v>
+        <v>30.54000000000002</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>52</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
@@ -74255,10 +74255,10 @@
         </is>
       </c>
       <c r="B5" s="6" t="n">
-        <v>34.21000000000004</v>
+        <v>27.46000000000004</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>32</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
@@ -74268,10 +74268,10 @@
         </is>
       </c>
       <c r="B6" s="6" t="n">
-        <v>38.45000000000005</v>
+        <v>25.96000000000004</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>18</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
@@ -74281,10 +74281,10 @@
         </is>
       </c>
       <c r="B7" s="6" t="n">
-        <v>38.60000000000002</v>
+        <v>25.25</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>16</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8">
@@ -74294,10 +74294,10 @@
         </is>
       </c>
       <c r="B8" s="6" t="n">
-        <v>33.01000000000005</v>
+        <v>24.77000000000004</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>36</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
@@ -74307,10 +74307,10 @@
         </is>
       </c>
       <c r="B9" s="6" t="n">
-        <v>29.94</v>
+        <v>24.82000000000005</v>
       </c>
       <c r="C9" s="6" t="n">
-        <v>47</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
@@ -74433,7 +74433,7 @@
         <v/>
       </c>
       <c r="D2" s="6" t="n">
-        <v>211</v>
+        <v>540</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>40</v>
@@ -74445,19 +74445,19 @@
         <v>3.5</v>
       </c>
       <c r="H2" s="6" t="n">
-        <v>0.258089486500438</v>
+        <v>0.2021933172147277</v>
       </c>
       <c r="I2" s="6" t="n">
-        <v>26.13139255483264</v>
+        <v>24.99901900503886</v>
       </c>
       <c r="J2" s="6" t="n">
-        <v>59.04176874119141</v>
+        <v>82.75220005551931</v>
       </c>
       <c r="K2" s="6" t="n">
-        <v>29.77837247865193</v>
+        <v>25.13998536761977</v>
       </c>
       <c r="L2" s="6" t="n">
-        <v>61.83652783916449</v>
+        <v>92.62720674782489</v>
       </c>
       <c r="M2" s="6" t="n">
         <v>1.448572791205265</v>
@@ -74477,10 +74477,10 @@
         <v/>
       </c>
       <c r="D3" s="6" t="n">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>6</v>
@@ -74489,19 +74489,19 @@
         <v>3.5</v>
       </c>
       <c r="H3" s="6" t="n">
-        <v>0.2398282444603726</v>
+        <v>0.1451270753495023</v>
       </c>
       <c r="I3" s="6" t="n">
-        <v>26.7331927377835</v>
+        <v>27.56653150812798</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>63.68531215673152</v>
+        <v>72.44192286071458</v>
       </c>
       <c r="K3" s="6" t="n">
-        <v>29.82513760553257</v>
+        <v>29.85232199807365</v>
       </c>
       <c r="L3" s="6" t="n">
-        <v>61.83652783916449</v>
+        <v>30.91826391958224</v>
       </c>
       <c r="M3" s="6" t="n">
         <v>1.448572791205265</v>
@@ -74521,31 +74521,31 @@
         <v/>
       </c>
       <c r="D4" s="6" t="n">
-        <v>210</v>
+        <v>115</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4" s="6" t="n">
         <v>3.5</v>
       </c>
       <c r="H4" s="6" t="n">
-        <v>0.2765140945606088</v>
+        <v>0.04300218633117147</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>25.52137885854142</v>
+        <v>26.84686117907648</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>54.37935313131648</v>
+        <v>71.76896877984869</v>
       </c>
       <c r="K4" s="6" t="n">
-        <v>29.73083743188079</v>
+        <v>29.70008554679049</v>
       </c>
       <c r="L4" s="6" t="n">
-        <v>61.83652783916449</v>
+        <v>0</v>
       </c>
       <c r="M4" s="6" t="n">
         <v>1.448572791205265</v>
@@ -74565,7 +74565,7 @@
         <v/>
       </c>
       <c r="D5" s="6" t="n">
-        <v>316</v>
+        <v>540</v>
       </c>
       <c r="E5" s="6" t="n">
         <v>40</v>
@@ -74577,19 +74577,19 @@
         <v>3.5</v>
       </c>
       <c r="H5" s="6" t="n">
-        <v>0.3054575913542633</v>
+        <v>0.2021933172147277</v>
       </c>
       <c r="I5" s="6" t="n">
-        <v>27.595405452374</v>
+        <v>24.99901900503886</v>
       </c>
       <c r="J5" s="6" t="n">
-        <v>44.31824531656468</v>
+        <v>82.75220005551931</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>34.43261610577463</v>
+        <v>25.13998536761977</v>
       </c>
       <c r="L5" s="6" t="n">
-        <v>30.9558712909312</v>
+        <v>92.62720674782489</v>
       </c>
       <c r="M5" s="6" t="n">
         <v>1.448572791205265</v>
@@ -74609,31 +74609,31 @@
         <v/>
       </c>
       <c r="D6" s="6" t="n">
-        <v>325</v>
+        <v>540</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G6" s="6" t="n">
         <v>3.5</v>
       </c>
       <c r="H6" s="6" t="n">
-        <v>0.1340229276082507</v>
+        <v>0.2021933172147277</v>
       </c>
       <c r="I6" s="6" t="n">
-        <v>30.3483044843187</v>
+        <v>24.99901900503886</v>
       </c>
       <c r="J6" s="6" t="n">
-        <v>43.03157929114731</v>
+        <v>82.75220005551931</v>
       </c>
       <c r="K6" s="6" t="n">
-        <v>39.08333401772904</v>
+        <v>25.13998536761977</v>
       </c>
       <c r="L6" s="6" t="n">
-        <v>0</v>
+        <v>92.62720674782489</v>
       </c>
       <c r="M6" s="6" t="n">
         <v>1.448572791205265</v>
@@ -74653,31 +74653,31 @@
         <v/>
       </c>
       <c r="D7" s="6" t="n">
-        <v>325</v>
+        <v>540</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G7" s="6" t="n">
         <v>3.5</v>
       </c>
       <c r="H7" s="6" t="n">
-        <v>0.1340229276082507</v>
+        <v>0.2021933172147277</v>
       </c>
       <c r="I7" s="6" t="n">
-        <v>30.3483044843187</v>
+        <v>24.99901900503886</v>
       </c>
       <c r="J7" s="6" t="n">
-        <v>43.03157929114731</v>
+        <v>82.75220005551931</v>
       </c>
       <c r="K7" s="6" t="n">
-        <v>39.08333401772904</v>
+        <v>25.13998536761977</v>
       </c>
       <c r="L7" s="6" t="n">
-        <v>0</v>
+        <v>92.62720674782489</v>
       </c>
       <c r="M7" s="6" t="n">
         <v>1.448572791205265</v>
@@ -74697,7 +74697,7 @@
         <v/>
       </c>
       <c r="D8" s="6" t="n">
-        <v>316</v>
+        <v>540</v>
       </c>
       <c r="E8" s="6" t="n">
         <v>40</v>
@@ -74709,19 +74709,19 @@
         <v>3.5</v>
       </c>
       <c r="H8" s="6" t="n">
-        <v>0.3054575913542633</v>
+        <v>0.2021933172147277</v>
       </c>
       <c r="I8" s="6" t="n">
-        <v>27.595405452374</v>
+        <v>24.99901900503886</v>
       </c>
       <c r="J8" s="6" t="n">
-        <v>44.31824531656468</v>
+        <v>82.75220005551931</v>
       </c>
       <c r="K8" s="6" t="n">
-        <v>34.43261610577463</v>
+        <v>25.13998536761977</v>
       </c>
       <c r="L8" s="6" t="n">
-        <v>30.9558712909312</v>
+        <v>92.62720674782489</v>
       </c>
       <c r="M8" s="6" t="n">
         <v>1.448572791205265</v>
@@ -74741,7 +74741,7 @@
         <v/>
       </c>
       <c r="D9" s="6" t="n">
-        <v>209</v>
+        <v>540</v>
       </c>
       <c r="E9" s="6" t="n">
         <v>40</v>
@@ -74753,19 +74753,19 @@
         <v>3.5</v>
       </c>
       <c r="H9" s="6" t="n">
-        <v>0.2951059607561097</v>
+        <v>0.2021933172147277</v>
       </c>
       <c r="I9" s="6" t="n">
-        <v>24.90291149916732</v>
+        <v>24.99901900503886</v>
       </c>
       <c r="J9" s="6" t="n">
-        <v>49.69749474388039</v>
+        <v>82.75220005551931</v>
       </c>
       <c r="K9" s="6" t="n">
-        <v>29.68251493686915</v>
+        <v>25.13998536761977</v>
       </c>
       <c r="L9" s="6" t="n">
-        <v>61.83652783916449</v>
+        <v>92.62720674782489</v>
       </c>
       <c r="M9" s="6" t="n">
         <v>1.448572791205265</v>

</xml_diff>